<commit_message>
Can update a form from XLSX file.
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="5900" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample" sheetId="1" r:id="rId1"/>
+    <sheet name="list" sheetId="1" r:id="rId1"/>
+    <sheet name="sample data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>KEY</t>
   </si>
@@ -55,13 +56,28 @@
   </si>
   <si>
     <t>098765</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>root@localhost.localdomain</t>
+  </si>
+  <si>
+    <t>unsecure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -73,6 +89,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,16 +119,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -517,4 +544,54 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>